<commit_message>
Fix schedule course generation bug
</commit_message>
<xml_diff>
--- a/static/schedule-courses/Horario 1-2024 - 2559202.xlsx
+++ b/static/schedule-courses/Horario 1-2024 - 2559202.xlsx
@@ -659,28 +659,28 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
@@ -702,28 +702,28 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico 
+          <t>Proyecto 2  + Manual Técnico 
  ALVARO PEREZ NIÑO 
  703</t>
         </is>
@@ -995,7 +995,7 @@
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>Proyecto 2 + Manual Técnico</t>
+          <t>Proyecto 2  + Manual Técnico</t>
         </is>
       </c>
       <c r="B28" s="6" t="inlineStr">

</xml_diff>